<commit_message>
20th dec 24 TC design
</commit_message>
<xml_diff>
--- a/TestData/6thJuly Selenium.xlsx
+++ b/TestData/6thJuly Selenium.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\6th July 2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\6th July 2024\Workspace\6thJuly_Framework_MavenProject\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F846D7C-A05A-425A-A098-87870180FBB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{554213D0-BD1F-49D6-B23D-3769522CFAF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="35">
   <si>
     <t>abc1</t>
   </si>
@@ -134,13 +134,16 @@
   </si>
   <si>
     <t xml:space="preserve">2nd execution </t>
+  </si>
+  <si>
+    <t>Sauce Labs Onesie</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,6 +156,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF171D1E"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="2">
@@ -190,10 +200,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -695,10 +706,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A3D3299-4839-4B22-B931-C162B8635706}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -720,13 +731,23 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>7.99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B17" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C17" t="s">
         <v>15</v>
       </c>
     </row>
@@ -968,7 +989,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48BBC670-3A7E-424D-8488-C2DFD67B6DB0}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>

</xml_diff>